<commit_message>
adding capability of discarding timestamps
</commit_message>
<xml_diff>
--- a/sorted_data.xlsx
+++ b/sorted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,31 +433,118 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="3"/>
     <row r="4"/>
     <row r="5">
       <c r="A5" t="n">
         <v>34</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>25</v>
-      </c>
-    </row>
+    <row r="6"/>
     <row r="7"/>
     <row r="8">
       <c r="A8" t="n">
         <v>89</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>7</v>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">L: </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22"/>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25"/>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>R:</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31"/>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34"/>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lever data added to single-cell lists to copy paste.
</commit_message>
<xml_diff>
--- a/sorted_data.xlsx
+++ b/sorted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A46"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -657,6 +657,34 @@
         <v>808.16</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>L:</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>16.99, 36.01, 68.54, 40.2, 54.79, 57.88, 42.47, 24.88, 2.47, 10.08, 34.11, 41.02, 6.64, 4.67, 5.87, 41.34, 161.88, 38.19, 69.9, 6.19, 40.93, 139.26, 2239.9, 843.3, 53.45, 97.99, 1582.14, 32.07, 33.6, 68.14, 33, 70.51, 640.75, 54.36, 47.21</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>R:</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>330.4, 154.07, 217.84, 105.83, 5182.37, 1.04, 808.16</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Formatting and data processing correct - current working version.
</commit_message>
<xml_diff>
--- a/sorted_data.xlsx
+++ b/sorted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,186 +439,301 @@
           <t>L:</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Running Total</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>16.99</v>
       </c>
+      <c r="B4" t="n">
+        <v>16.99</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>36.01</v>
       </c>
+      <c r="B5" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>68.54000000000001</v>
       </c>
+      <c r="B6" t="n">
+        <v>121.54</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>40.2</v>
       </c>
+      <c r="B7" t="n">
+        <v>161.74</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>54.79</v>
       </c>
+      <c r="B8" t="n">
+        <v>216.53</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>57.88</v>
       </c>
+      <c r="B9" t="n">
+        <v>274.41</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>42.47</v>
       </c>
+      <c r="B10" t="n">
+        <v>316.88</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>24.88</v>
       </c>
+      <c r="B11" t="n">
+        <v>341.76</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>2.47</v>
       </c>
+      <c r="B12" t="n">
+        <v>344.23</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>10.08</v>
       </c>
+      <c r="B13" t="n">
+        <v>354.31</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>34.11</v>
       </c>
+      <c r="B14" t="n">
+        <v>388.42</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>41.02</v>
       </c>
+      <c r="B15" t="n">
+        <v>429.44</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>6.64</v>
       </c>
+      <c r="B16" t="n">
+        <v>436.08</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>4.67</v>
       </c>
+      <c r="B17" t="n">
+        <v>440.75</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>5.87</v>
       </c>
+      <c r="B18" t="n">
+        <v>446.62</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>41.34</v>
       </c>
+      <c r="B19" t="n">
+        <v>487.96</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>161.88</v>
       </c>
+      <c r="B20" t="n">
+        <v>649.84</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>38.19</v>
       </c>
+      <c r="B21" t="n">
+        <v>688.03</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>69.90000000000001</v>
       </c>
+      <c r="B22" t="n">
+        <v>757.9299999999999</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>6.19</v>
       </c>
+      <c r="B23" t="n">
+        <v>764.12</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>40.93</v>
       </c>
+      <c r="B24" t="n">
+        <v>805.05</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>139.26</v>
       </c>
+      <c r="B25" t="n">
+        <v>944.3099999999999</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>2239.9</v>
       </c>
+      <c r="B26" t="n">
+        <v>3184.21</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
         <v>843.3</v>
       </c>
+      <c r="B27" t="n">
+        <v>4027.51</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>53.45</v>
       </c>
+      <c r="B28" t="n">
+        <v>4080.96</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>97.98999999999999</v>
       </c>
+      <c r="B29" t="n">
+        <v>4178.95</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>1582.14</v>
       </c>
+      <c r="B30" t="n">
+        <v>5761.09</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>32.07</v>
       </c>
+      <c r="B31" t="n">
+        <v>5793.16</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>33.6</v>
       </c>
+      <c r="B32" t="n">
+        <v>5826.76</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>68.14</v>
       </c>
+      <c r="B33" t="n">
+        <v>5894.900000000001</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>33</v>
       </c>
+      <c r="B34" t="n">
+        <v>5927.900000000001</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>70.51000000000001</v>
       </c>
+      <c r="B35" t="n">
+        <v>5998.410000000001</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>640.75</v>
       </c>
+      <c r="B36" t="n">
+        <v>6639.160000000001</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
         <v>54.36</v>
       </c>
+      <c r="B37" t="n">
+        <v>6693.52</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>47.21</v>
       </c>
+      <c r="B38" t="n">
+        <v>6740.73</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
           <t>R:</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Running Total</t>
         </is>
       </c>
     </row>
@@ -626,41 +741,62 @@
       <c r="A40" t="n">
         <v>330.4</v>
       </c>
+      <c r="B40" t="n">
+        <v>330.4</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
         <v>154.07</v>
       </c>
+      <c r="B41" t="n">
+        <v>484.47</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
         <v>217.84</v>
       </c>
+      <c r="B42" t="n">
+        <v>702.3099999999999</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>105.83</v>
       </c>
+      <c r="B43" t="n">
+        <v>808.14</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
         <v>5182.37</v>
       </c>
+      <c r="B44" t="n">
+        <v>5990.51</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
         <v>1.04</v>
       </c>
+      <c r="B45" t="n">
+        <v>5991.55</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
         <v>808.16</v>
       </c>
+      <c r="B46" t="n">
+        <v>6799.71</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>L:</t>
+          <t>L ~ Raw</t>
         </is>
       </c>
     </row>
@@ -674,7 +810,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>R:</t>
+          <t>R ~ Raw</t>
         </is>
       </c>
     </row>
@@ -682,6 +818,34 @@
       <c r="A50" t="inlineStr">
         <is>
           <t>330.4, 154.07, 217.84, 105.83, 5182.37, 1.04, 808.16</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>L ~ Running Totals</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>16.99, 53.0, 121.54, 161.74, 216.53, 274.41, 316.88, 341.76, 344.23, 354.31, 388.42, 429.44, 436.08, 440.75, 446.62, 487.96000000000004, 649.84, 688.03, 757.93, 764.12, 805.05, 944.31, 3184.21, 4027.51, 4080.96, 4178.95, 5761.09, 5793.16, 5826.76, 5894.900000000001, 5927.900000000001, 5998.410000000001, 6639.160000000001, 6693.52, 6740.7300000000005</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>R ~ Running Totals</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>330.4, 484.46999999999997, 702.31, 808.14, 5990.51, 5991.55, 6799.71</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
All features working, all formatting fixed
</commit_message>
<xml_diff>
--- a/sorted_data.xlsx
+++ b/sorted_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Running Total</t>
+          <t>L Totals</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> L Minutes</t>
         </is>
       </c>
     </row>
@@ -452,6 +457,9 @@
       <c r="B4" t="n">
         <v>16.99</v>
       </c>
+      <c r="C4" t="n">
+        <v>0.283</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -460,6 +468,9 @@
       <c r="B5" t="n">
         <v>53</v>
       </c>
+      <c r="C5" t="n">
+        <v>0.883</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -468,6 +479,9 @@
       <c r="B6" t="n">
         <v>121.54</v>
       </c>
+      <c r="C6" t="n">
+        <v>2.026</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -476,6 +490,9 @@
       <c r="B7" t="n">
         <v>161.74</v>
       </c>
+      <c r="C7" t="n">
+        <v>2.696</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -484,6 +501,9 @@
       <c r="B8" t="n">
         <v>216.53</v>
       </c>
+      <c r="C8" t="n">
+        <v>3.609</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -492,6 +512,9 @@
       <c r="B9" t="n">
         <v>274.41</v>
       </c>
+      <c r="C9" t="n">
+        <v>4.574</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -500,6 +523,9 @@
       <c r="B10" t="n">
         <v>316.88</v>
       </c>
+      <c r="C10" t="n">
+        <v>5.281</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -508,6 +534,9 @@
       <c r="B11" t="n">
         <v>341.76</v>
       </c>
+      <c r="C11" t="n">
+        <v>5.696</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -516,6 +545,9 @@
       <c r="B12" t="n">
         <v>344.23</v>
       </c>
+      <c r="C12" t="n">
+        <v>5.737</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -524,6 +556,9 @@
       <c r="B13" t="n">
         <v>354.31</v>
       </c>
+      <c r="C13" t="n">
+        <v>5.905</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -532,6 +567,9 @@
       <c r="B14" t="n">
         <v>388.42</v>
       </c>
+      <c r="C14" t="n">
+        <v>6.474</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -540,6 +578,9 @@
       <c r="B15" t="n">
         <v>429.44</v>
       </c>
+      <c r="C15" t="n">
+        <v>7.157</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -548,6 +589,9 @@
       <c r="B16" t="n">
         <v>436.08</v>
       </c>
+      <c r="C16" t="n">
+        <v>7.268</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -556,6 +600,9 @@
       <c r="B17" t="n">
         <v>440.75</v>
       </c>
+      <c r="C17" t="n">
+        <v>7.346</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -564,6 +611,9 @@
       <c r="B18" t="n">
         <v>446.62</v>
       </c>
+      <c r="C18" t="n">
+        <v>7.444</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -572,6 +622,9 @@
       <c r="B19" t="n">
         <v>487.96</v>
       </c>
+      <c r="C19" t="n">
+        <v>8.132999999999999</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -580,6 +633,9 @@
       <c r="B20" t="n">
         <v>649.84</v>
       </c>
+      <c r="C20" t="n">
+        <v>10.831</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -588,6 +644,9 @@
       <c r="B21" t="n">
         <v>688.03</v>
       </c>
+      <c r="C21" t="n">
+        <v>11.467</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -596,6 +655,9 @@
       <c r="B22" t="n">
         <v>757.9299999999999</v>
       </c>
+      <c r="C22" t="n">
+        <v>12.632</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -604,6 +666,9 @@
       <c r="B23" t="n">
         <v>764.12</v>
       </c>
+      <c r="C23" t="n">
+        <v>12.735</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -612,6 +677,9 @@
       <c r="B24" t="n">
         <v>805.05</v>
       </c>
+      <c r="C24" t="n">
+        <v>13.417</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -620,6 +688,9 @@
       <c r="B25" t="n">
         <v>944.3099999999999</v>
       </c>
+      <c r="C25" t="n">
+        <v>15.738</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -628,6 +699,9 @@
       <c r="B26" t="n">
         <v>3184.21</v>
       </c>
+      <c r="C26" t="n">
+        <v>53.07</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -636,6 +710,9 @@
       <c r="B27" t="n">
         <v>4027.51</v>
       </c>
+      <c r="C27" t="n">
+        <v>67.125</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -644,6 +721,9 @@
       <c r="B28" t="n">
         <v>4080.96</v>
       </c>
+      <c r="C28" t="n">
+        <v>68.01600000000001</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -652,6 +732,9 @@
       <c r="B29" t="n">
         <v>4178.95</v>
       </c>
+      <c r="C29" t="n">
+        <v>69.649</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -660,6 +743,9 @@
       <c r="B30" t="n">
         <v>5761.09</v>
       </c>
+      <c r="C30" t="n">
+        <v>96.018</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -668,6 +754,9 @@
       <c r="B31" t="n">
         <v>5793.16</v>
       </c>
+      <c r="C31" t="n">
+        <v>96.553</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -676,6 +765,9 @@
       <c r="B32" t="n">
         <v>5826.76</v>
       </c>
+      <c r="C32" t="n">
+        <v>97.113</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -684,6 +776,9 @@
       <c r="B33" t="n">
         <v>5894.900000000001</v>
       </c>
+      <c r="C33" t="n">
+        <v>98.248</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -692,6 +787,9 @@
       <c r="B34" t="n">
         <v>5927.900000000001</v>
       </c>
+      <c r="C34" t="n">
+        <v>98.798</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -700,6 +798,9 @@
       <c r="B35" t="n">
         <v>5998.410000000001</v>
       </c>
+      <c r="C35" t="n">
+        <v>99.974</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -708,6 +809,9 @@
       <c r="B36" t="n">
         <v>6639.160000000001</v>
       </c>
+      <c r="C36" t="n">
+        <v>110.653</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -716,6 +820,9 @@
       <c r="B37" t="n">
         <v>6693.52</v>
       </c>
+      <c r="C37" t="n">
+        <v>111.559</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -724,6 +831,9 @@
       <c r="B38" t="n">
         <v>6740.73</v>
       </c>
+      <c r="C38" t="n">
+        <v>112.346</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -733,7 +843,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Running Total</t>
+          <t>R Totals</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>R Minutes</t>
         </is>
       </c>
     </row>
@@ -744,6 +859,9 @@
       <c r="B40" t="n">
         <v>330.4</v>
       </c>
+      <c r="C40" t="n">
+        <v>0.283</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -752,6 +870,9 @@
       <c r="B41" t="n">
         <v>484.47</v>
       </c>
+      <c r="C41" t="n">
+        <v>0.883</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -760,6 +881,9 @@
       <c r="B42" t="n">
         <v>702.3099999999999</v>
       </c>
+      <c r="C42" t="n">
+        <v>2.026</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -768,6 +892,9 @@
       <c r="B43" t="n">
         <v>808.14</v>
       </c>
+      <c r="C43" t="n">
+        <v>2.696</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -776,6 +903,9 @@
       <c r="B44" t="n">
         <v>5990.51</v>
       </c>
+      <c r="C44" t="n">
+        <v>3.609</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -784,6 +914,9 @@
       <c r="B45" t="n">
         <v>5991.55</v>
       </c>
+      <c r="C45" t="n">
+        <v>4.574</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -792,6 +925,9 @@
       <c r="B46" t="n">
         <v>6799.71</v>
       </c>
+      <c r="C46" t="n">
+        <v>5.281</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -846,6 +982,34 @@
       <c r="A54" t="inlineStr">
         <is>
           <t>330.4, 484.46999999999997, 702.31, 808.14, 5990.51, 5991.55, 6799.71</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>L ~ Minutes</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>0.283, 1.166, 3.192, 5.888, 9.497, 14.07, 19.351, 25.047, 30.784, 36.689, 43.163, 50.32, 57.588, 64.934, 72.378, 80.511, 91.342, 102.809, 115.441, 128.176, 141.593, 157.331, 210.401, 277.526, 345.542, 415.191, 511.209, 607.762, 704.875, 803.123, 901.921, 1001.895, 1112.548, 1224.107, 1336.452</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>R ~ Minutes</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>5.507, 13.581, 25.286, 38.755, 138.597, 238.456, 351.784</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Formatting for right lever data single-cell string fixed
</commit_message>
<xml_diff>
--- a/sorted_data.xlsx
+++ b/sorted_data.xlsx
@@ -860,7 +860,7 @@
         <v>330.4</v>
       </c>
       <c r="C40" t="n">
-        <v>0.283</v>
+        <v>5.507</v>
       </c>
     </row>
     <row r="41">
@@ -871,7 +871,7 @@
         <v>484.47</v>
       </c>
       <c r="C41" t="n">
-        <v>0.883</v>
+        <v>8.074</v>
       </c>
     </row>
     <row r="42">
@@ -882,7 +882,7 @@
         <v>702.3099999999999</v>
       </c>
       <c r="C42" t="n">
-        <v>2.026</v>
+        <v>11.705</v>
       </c>
     </row>
     <row r="43">
@@ -893,7 +893,7 @@
         <v>808.14</v>
       </c>
       <c r="C43" t="n">
-        <v>2.696</v>
+        <v>13.469</v>
       </c>
     </row>
     <row r="44">
@@ -904,7 +904,7 @@
         <v>5990.51</v>
       </c>
       <c r="C44" t="n">
-        <v>3.609</v>
+        <v>99.842</v>
       </c>
     </row>
     <row r="45">
@@ -915,7 +915,7 @@
         <v>5991.55</v>
       </c>
       <c r="C45" t="n">
-        <v>4.574</v>
+        <v>99.85899999999999</v>
       </c>
     </row>
     <row r="46">
@@ -926,7 +926,7 @@
         <v>6799.71</v>
       </c>
       <c r="C46" t="n">
-        <v>5.281</v>
+        <v>113.329</v>
       </c>
     </row>
     <row r="47">
@@ -995,7 +995,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>0.283, 1.166, 3.192, 5.888, 9.497, 14.07, 19.351, 25.047, 30.784, 36.689, 43.163, 50.32, 57.588, 64.934, 72.378, 80.511, 91.342, 102.809, 115.441, 128.176, 141.593, 157.331, 210.401, 277.526, 345.542, 415.191, 511.209, 607.762, 704.875, 803.123, 901.921, 1001.895, 1112.548, 1224.107, 1336.452</t>
+          <t>0.283, 0.883, 2.026, 2.696, 3.609, 4.574, 5.281, 5.696, 5.737, 5.905, 6.474, 7.157, 7.268, 7.346, 7.444, 8.133, 10.831, 11.467, 12.632, 12.735, 13.417, 15.738, 53.07, 67.125, 68.016, 69.649, 96.018, 96.553, 97.113, 98.248, 98.798, 99.974, 110.653, 111.559, 112.346</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5.507, 13.581, 25.286, 38.755, 138.597, 238.456, 351.784</t>
+          <t>5.507, 8.074, 11.705, 13.469, 99.842, 99.859, 113.329</t>
         </is>
       </c>
     </row>

</xml_diff>